<commit_message>
BUGFIX #i04 pipeline problem solved
Signed-off-by: JochenRust <49911366+JochenRust@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ISSUES.xlsx
+++ b/ISSUES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\sorngen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD3A58A-8BBF-4D11-A3CD-054D8B4C9CE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F113E3B-3F60-4B53-B879-FD703B41FE3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="984" yWindow="2088" windowWidth="19836" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -662,7 +662,7 @@
   <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -763,7 +763,7 @@
         <v>41</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>53</v>

</xml_diff>

<commit_message>
Output of FunctionTable Generator added Signed-off-by: JochenRust <49911366+JochenRust@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ISSUES.xlsx
+++ b/ISSUES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\sorngen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F113E3B-3F60-4B53-B879-FD703B41FE3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA38469-6F79-4E53-A8B8-0D8C6B470049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="984" yWindow="2088" windowWidth="19836" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="60">
   <si>
     <t>Severity</t>
   </si>
@@ -185,9 +185,6 @@
   </si>
   <si>
     <t>Bad labeling of arithmetic units</t>
-  </si>
-  <si>
-    <t>appears when pipeline parameter is not zero</t>
   </si>
   <si>
     <t>Reproducable in kinematik.sorn</t>
@@ -204,6 +201,12 @@
   <si>
     <t>SST dictonary registration added in ternary merge function (design_elaborator.py, line261)
 SST node replace has been adapted to ternary nodes, hanlding of 3rd sibling has been added (type_SST.py, line 170)</t>
+  </si>
+  <si>
+    <t>Register Insertion for full design (Toplevel-oriented)</t>
+  </si>
+  <si>
+    <t>maxDepth parameter of SST has been changed to depth when accessed in the insertRegister function</t>
   </si>
 </sst>
 </file>
@@ -661,8 +664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -712,7 +715,7 @@
         <v>47</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -751,7 +754,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="18"/>
       <c r="B6" s="19" t="s">
         <v>11</v>
@@ -766,7 +769,7 @@
         <v>47</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -784,7 +787,7 @@
         <v>43</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -802,7 +805,7 @@
         <v>43</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -811,7 +814,7 @@
         <v>14</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>40</v>
@@ -820,7 +823,7 @@
         <v>43</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -828,7 +831,9 @@
       <c r="B10" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="D10" s="2" t="s">
         <v>41</v>
       </c>

</xml_diff>